<commit_message>
Adding visualization of isolated observations per species
</commit_message>
<xml_diff>
--- a/output/Automatic_Labeling_Kyoogu/isolated_observations.xlsx
+++ b/output/Automatic_Labeling_Kyoogu/isolated_observations.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -477,7 +477,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -493,7 +493,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -509,7 +509,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -525,7 +525,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -541,7 +541,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -557,7 +557,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -589,7 +589,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -605,7 +605,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -621,7 +621,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -637,7 +637,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -653,7 +653,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -669,7 +669,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -685,7 +685,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>DEND</t>
+          <t>Dendropsophus_microcephalus</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -701,7 +701,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>TRGL</t>
+          <t>Troglodytes_aedon</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -717,7 +717,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -733,7 +733,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -749,7 +749,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -765,7 +765,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>MMLS</t>
+          <t>Alouatta_sp</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -797,7 +797,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MMLS</t>
+          <t>Alouatta_sp</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -813,7 +813,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -829,7 +829,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -845,7 +845,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -861,7 +861,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -877,7 +877,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -893,7 +893,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>MMLS</t>
+          <t>Alouatta_sp</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -909,7 +909,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -925,7 +925,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -941,7 +941,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -957,7 +957,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -973,7 +973,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -989,7 +989,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1005,7 +1005,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1053,7 +1053,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -1069,7 +1069,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -1133,7 +1133,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1149,7 +1149,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1165,7 +1165,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1181,7 +1181,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -1197,7 +1197,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1229,7 +1229,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1245,7 +1245,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -1277,7 +1277,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C54" t="n">
@@ -1309,7 +1309,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C55" t="n">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C56" t="n">
@@ -1341,7 +1341,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C57" t="n">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C58" t="n">
@@ -1373,7 +1373,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C59" t="n">
@@ -1389,7 +1389,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -1405,7 +1405,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C61" t="n">
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C62" t="n">
@@ -1437,7 +1437,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C63" t="n">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C64" t="n">
@@ -1469,7 +1469,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C65" t="n">
@@ -1485,7 +1485,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C66" t="n">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C67" t="n">
@@ -1517,7 +1517,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C68" t="n">
@@ -1533,7 +1533,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C69" t="n">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C70" t="n">
@@ -1565,7 +1565,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C71" t="n">
@@ -1581,7 +1581,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -1597,7 +1597,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C73" t="n">
@@ -1613,7 +1613,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C74" t="n">
@@ -1629,7 +1629,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C75" t="n">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C77" t="n">
@@ -1677,7 +1677,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C78" t="n">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C79" t="n">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C80" t="n">
@@ -1725,7 +1725,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C81" t="n">
@@ -1741,7 +1741,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C82" t="n">
@@ -1757,7 +1757,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C83" t="n">
@@ -1773,7 +1773,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C84" t="n">
@@ -1789,7 +1789,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C85" t="n">
@@ -1805,7 +1805,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C86" t="n">
@@ -1821,7 +1821,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C87" t="n">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C88" t="n">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1869,7 +1869,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1885,7 +1885,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C91" t="n">
@@ -1901,7 +1901,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C92" t="n">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C93" t="n">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C94" t="n">
@@ -1949,7 +1949,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C95" t="n">
@@ -1965,7 +1965,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C96" t="n">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C97" t="n">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C98" t="n">
@@ -2013,7 +2013,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C99" t="n">
@@ -2029,7 +2029,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C100" t="n">
@@ -2045,7 +2045,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>MMLS</t>
+          <t>Alouatta_sp</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2077,7 +2077,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>MMLS</t>
+          <t>Alouatta_sp</t>
         </is>
       </c>
       <c r="C103" t="n">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>PTGN</t>
+          <t>Patagioenas_cayennensis</t>
         </is>
       </c>
       <c r="C104" t="n">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C105" t="n">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>FUSC</t>
+          <t>Leptodactylus_fuscus</t>
         </is>
       </c>
       <c r="C106" t="n">
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>BOAN</t>
+          <t>Boana_platanera</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>DDPX</t>
+          <t>Dendroplex_picus</t>
         </is>
       </c>
       <c r="C108" t="n">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>FRAG</t>
+          <t>Leptodactylus_fragilis</t>
         </is>
       </c>
       <c r="C109" t="n">

</xml_diff>